<commit_message>
1. added data points 2. improved charts with original and interpolated figures
</commit_message>
<xml_diff>
--- a/data/BabyWeights.xlsx
+++ b/data/BabyWeights.xlsx
@@ -384,7 +384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
@@ -418,7 +418,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A46" si="0">1+A3</f>
+        <f t="shared" ref="A4:A42" si="0">1+A3</f>
         <v>44756</v>
       </c>
     </row>
@@ -672,28 +672,70 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
+      <c r="A35" s="1">
+        <f t="shared" si="0"/>
+        <v>44787</v>
+      </c>
+      <c r="B35" s="2">
+        <v>4255</v>
+      </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
+      <c r="A36" s="1">
+        <f t="shared" si="0"/>
+        <v>44788</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
+      <c r="A37" s="1">
+        <f t="shared" si="0"/>
+        <v>44789</v>
+      </c>
+      <c r="B37" s="2">
+        <v>4315</v>
+      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
+      <c r="A38" s="1">
+        <f t="shared" si="0"/>
+        <v>44790</v>
+      </c>
+      <c r="B38" s="2">
+        <v>4335</v>
+      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
+      <c r="A39" s="1">
+        <f t="shared" si="0"/>
+        <v>44791</v>
+      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
+      <c r="A40" s="1">
+        <f t="shared" si="0"/>
+        <v>44792</v>
+      </c>
+      <c r="B40" s="2">
+        <v>4425</v>
+      </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
+      <c r="A41" s="1">
+        <f t="shared" si="0"/>
+        <v>44793</v>
+      </c>
+      <c r="B41" s="2">
+        <v>4450</v>
+      </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
+      <c r="A42" s="1">
+        <f t="shared" si="0"/>
+        <v>44794</v>
+      </c>
+      <c r="B42" s="2">
+        <v>4545</v>
+      </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>

</xml_diff>